<commit_message>
Fine tuning, refactoring, analysis routine
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0AD065AC-8E6A-4B29-B7E5-515097537DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2144E01-0F23-4D98-811A-325B6CCCB011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>de</t>
   </si>
@@ -315,12 +315,6 @@
     <t>Lore Ipsum</t>
   </si>
   <si>
-    <t>THANKS</t>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
     <t>AGAIN</t>
   </si>
   <si>
@@ -341,6 +335,24 @@
   <si>
     <t xml:space="preserve">How many tones can you hear?\\ Your task is again  **to count only the tones heard**  and to enter the numerical value in the text field.  **You ignore the noise and don't count it**.
 </t>
+  </si>
+  <si>
+    <t>Entschuldigung!</t>
+  </si>
+  <si>
+    <t>Sorry!</t>
+  </si>
+  <si>
+    <t>STOP_HEAD</t>
+  </si>
+  <si>
+    <t>STOP_TEXT</t>
+  </si>
+  <si>
+    <t>Your listening device is not suitable for this test.</t>
+  </si>
+  <si>
+    <t>Ihr Abhörgerät ist leider nicht geeignet für diesen Test.</t>
   </si>
 </sst>
 </file>
@@ -700,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +819,7 @@
         <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -818,7 +830,7 @@
         <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -829,23 +841,23 @@
         <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>60</v>
@@ -1098,35 +1110,35 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New stop page text
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2144E01-0F23-4D98-811A-325B6CCCB011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2216D4E2-CE21-4AC3-B2C4-C6484DC836E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -337,22 +337,24 @@
 </t>
   </si>
   <si>
-    <t>Entschuldigung!</t>
-  </si>
-  <si>
-    <t>Sorry!</t>
-  </si>
-  <si>
     <t>STOP_HEAD</t>
   </si>
   <si>
     <t>STOP_TEXT</t>
   </si>
   <si>
-    <t>Your listening device is not suitable for this test.</t>
-  </si>
-  <si>
-    <t>Ihr Abhörgerät ist leider nicht geeignet für diesen Test.</t>
+    <t>Liebe:r Teilnehmer:in,</t>
+  </si>
+  <si>
+    <t>Dear participant,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the interview has ended. This can have several reasons:&lt;ol&gt;&lt;li&gt;Sufficient test persons with a similar playback device have already participated.&lt;/li&gt;&lt;li&gt; Your playback device is not part of our target group.&lt;/li&gt;&lt;/ol&gt;Since future studies may require more subjects and different target groups, we would be happy to see you again in the next study.\\Thank you for your interest and participation.
+</t>
+  </si>
+  <si>
+    <t>die Befragung wurde beendet. Das kann mehrere Gründe haben:&lt;ol&gt;&lt;li&gt;Es haben bereits genügend Probanden mit einem ähnlichen Wiedergabegerät teilgenommen.&lt;/li&gt;&lt;li&gt; Ihr Wiedergabegerät ist nicht Teil unserer Zielgruppe.&lt;/li&gt;
+&lt;/ol&gt;Da zukünftige Untersuchungen vielleicht mehr Probanden und andere Zielgruppen erfordern, würden wir uns freuen, Sie in der nächsten Studie wieder begrüßen zu können. \\Wir bedanken uns für Ihr Interesse und Ihre Teilnahme.</t>
   </si>
 </sst>
 </file>
@@ -1110,23 +1112,23 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small typo in dict
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2405D441-91D8-4948-BE30-41F147807A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5907F356-1E4A-4330-A372-9871B716861D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1530" windowWidth="27675" windowHeight="12495" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -369,10 +369,10 @@
     <t>Seite {{page_no}} von {{num_pages}}</t>
   </si>
   <si>
-    <t>Page {{question_no}} of {{num_questions}}</t>
-  </si>
-  <si>
     <t>Langsam von links nach rechts</t>
+  </si>
+  <si>
+    <t>Page {{page_no}} of {{num_pages}}</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +946,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
@@ -1169,7 +1169,7 @@
         <v>110</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New version 0.9.0 as per specification
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5907F356-1E4A-4330-A372-9871B716861D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF6C2D0-BB3D-464A-BAC4-A8A9DB963B07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1530" windowWidth="27675" windowHeight="12495" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="27495" windowHeight="12495" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
   <si>
     <t>de</t>
   </si>
@@ -373,6 +373,115 @@
   </si>
   <si>
     <t>Page {{page_no}} of {{num_pages}}</t>
+  </si>
+  <si>
+    <t>THLT_0013_PROMPT</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Which sound is the softest?&lt;/h4&gt;
+When you click the play button, you will hear an audio sample with three tones. These tones are separated by short pauses. You should indicate the quietest tone.</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Welcher Ton ist am leisesten?&lt;/h4&gt;Wenn Sie auf den Play-Button klicken, hören Sie ein Audiobeispiel in dem drei Töne zu hören sind. Diese Töne sind durch kurze Pausen getrennt. Sie sollen angeben, welcher Ton für Sie am leisesten klang.</t>
+  </si>
+  <si>
+    <t>THLT_0013_CHOICES1</t>
+  </si>
+  <si>
+    <t>THLT_0013_CHOICES2</t>
+  </si>
+  <si>
+    <t>THLT_0013_CHOICES3</t>
+  </si>
+  <si>
+    <t>FIRST sound is the SOFTEST</t>
+  </si>
+  <si>
+    <t>SECOND sound is the SOFTEST</t>
+  </si>
+  <si>
+    <t>THIRD sound is the SOFTEST</t>
+  </si>
+  <si>
+    <t>Der ERSTE Ton is am LEISESTEN</t>
+  </si>
+  <si>
+    <t>Der ZWEIT Ton is am LEISESTEN</t>
+  </si>
+  <si>
+    <t>Der DRITTE Ton is am LEISESTEN</t>
+  </si>
+  <si>
+    <t>SCC_PROMPT</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Kopfhörer zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Kopfhörern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmern wirklich Kopfhörer getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Kopfhörer zu tragen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Kopfhörer tragen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You indicated that you are using a device different from headphones to reproduce sound. However, the use of headphones is a basic requirement for this survey.&lt;/p&gt;&lt;p&gt;We integrated special listening tasks in the further course of the questionnaire. These tasks check whether the participants are actually wearing headphones. &lt;/p&gt;&lt;p&gt;We therefore ask you &lt;strong&gt; to wear headphones from now on&lt;/strong&gt; to successfully complete the survey. If you do not wear headphones from now on, you will be automatically screened out during the survey. Given the length of the questionnaire, this would be a pity.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Which device do you use to play back the sound in this survey?&lt;/p&gt;&lt;p&gt;Example: If you are using a smartphone that you have connected to headphones, you must select „headphones“.&lt;/p&gt;&lt;p&gt;Select the answer option that best describes your device.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Über welches Gerät geben Sie den Ton in dieser Befragung wieder? &lt;/p&gt;&lt;p&gt;Beispiel: Wenn Sie ein Smartphone benutzen, das Sie mit Kopfhörer verbunden haben, dann müssen Sie „Kopfhörer“ auswählen.&lt;/p&gt;&lt;p&gt;Wählen Sie das am ehesten Zutreffende aus.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>DEVICE_PROMPT</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE1</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE2</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE3</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE4</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE5</t>
+  </si>
+  <si>
+    <t>DEVICE_CHOICE6</t>
+  </si>
+  <si>
+    <t>Headphones</t>
+  </si>
+  <si>
+    <t>Laptop (built-in speakers)</t>
+  </si>
+  <si>
+    <t>Freestanding loudspeaker boxes</t>
+  </si>
+  <si>
+    <t>Smartphone (built-in speakers)</t>
+  </si>
+  <si>
+    <t>Tablet (built-in speakers)</t>
+  </si>
+  <si>
+    <t>Monitor/TV (built-in speakers)</t>
+  </si>
+  <si>
+    <t>Kopfhörer</t>
+  </si>
+  <si>
+    <t>Laptop (integrierte Lautsprecher)</t>
+  </si>
+  <si>
+    <t>Freistehende Lautsprecherboxen</t>
+  </si>
+  <si>
+    <t>Smartphone (integrierte Lautsprecher)</t>
+  </si>
+  <si>
+    <t>Tablet (integrierte Lautsprecher)</t>
+  </si>
+  <si>
+    <t>Monitor/TV (integrierte Lautsprecher)</t>
   </si>
 </sst>
 </file>
@@ -408,12 +517,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -730,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,180 +1122,312 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>113</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>122</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>123</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of rework
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF6C2D0-BB3D-464A-BAC4-A8A9DB963B07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58ECD69-23C4-4520-B46D-CC7F2936E96C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="27495" windowHeight="12495" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="1305" yWindow="2340" windowWidth="27495" windowHeight="12495" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="152">
   <si>
     <t>de</t>
   </si>
@@ -412,9 +412,6 @@
     <t>Der DRITTE Ton is am LEISESTEN</t>
   </si>
   <si>
-    <t>SCC_PROMPT</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Kopfhörer zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Kopfhörern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmern wirklich Kopfhörer getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Kopfhörer zu tragen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Kopfhörer tragen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
   </si>
   <si>
@@ -482,6 +479,18 @@
   </si>
   <si>
     <t>Monitor/TV (integrierte Lautsprecher)</t>
+  </si>
+  <si>
+    <t>SCC_PROMPT_LS</t>
+  </si>
+  <si>
+    <t>SCC_PROMPT_HP</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Lautsprecher zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Lautsprechern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmern wirklich Lautsprecher getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Lautsprecher zu benutzen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Lautsprecher benutzen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You indicated that you are using a device different from loudspeakers to reproduce sound. However, the use of loudspeakers is a basic requirement for this survey.&lt;/p&gt;&lt;p&gt;We integrated special listening tasks in the further course of the questionnaire. These tasks check whether the participants are actually using loudspeakers. &lt;/p&gt;&lt;p&gt;We therefore ask you &lt;strong&gt; to use loudspeakers from now on&lt;/strong&gt; to successfully complete the survey. If you do not use loudspeakers from now on, you will be automatically screened out during the survey. Given the length of the questionnaire, this would be a pity.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -845,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,90 +1353,101 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>142</v>
+      <c r="B53" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes according to specification 2021_12_02 (volume level, change of stimuli)
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yveswycisk/Library/Mobile Documents/com~apple~CloudDocs/HALT 2020/Veröffentlichung/Prozedur/Rohdaten - Fragen und Stimuli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yveswycisk/Library/Mobile Documents/com~apple~CloudDocs/HALT 2020/Veröffentlichung/Prozedur/Rohdaten - Fragen und Stimuli/V12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A58A92D-74F1-3344-B3DB-0581534EBAC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1649FDEB-D676-8843-B1CA-1C0C42D613A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21020" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -441,9 +441,6 @@
     <t>&lt;h4&gt;Wie viele Töne können Sie hören?&lt;/h4&gt;Wenn Sie auf den Play-Button klicken, hören Sie kurze Rauschabschnitte in regelmäßigen Abständen. Neben dem Rauschen sind auch Töne zu hören, die jedoch nie gleichzeitig mit dem Rauschen erklingen. Bitte **zählen Sie nur die gehörten Töne** und tragen Sie den Zahlenwert in das Textfeld ein. **Das Rauschen lassen Sie dabei unbeachtet und zählen es auch nicht mit**.</t>
   </si>
   <si>
-    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;When you click the play button, you will hear short noise events at regular intervals. In addition to the noise, tones are present. Tones and noise never sound simultaneously. Please **count only the tones heard** and enter the numerical value in the input box. **You should ignore the noise and don't count it**.</t>
-  </si>
-  <si>
     <t>&lt;h4&gt;Wie viele Töne können Sie hören?&lt;/h4&gt;Ihre Aufgabe ist es wieder, **nur die gehörten Töne zu zählen** und den Zahlenwert in das Textfeld einzutragen. **Das Rauschen lassen Sie dabei unbeachtet und zählen es auch nicht mit**.</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>Der Ton wandert von links nach rechts und anschließend wieder zurück nach links.</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;When you click the play button, you will hear short noise events at regular intervals. In addition to the noise, tones are present. Tones and noise never sound simultaneously. Please **count only the tones heard** and enter the numerical value in the input box. **You should ignore the noise and not count it**.</t>
   </si>
 </sst>
 </file>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -909,7 +909,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -920,7 +920,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -953,7 +953,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -964,7 +964,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -972,21 +972,21 @@
         <v>134</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -994,10 +994,10 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -1060,7 +1060,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1071,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1093,7 +1093,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
@@ -1112,10 +1112,10 @@
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1123,10 +1123,10 @@
         <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1134,13 +1134,13 @@
         <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
@@ -1156,10 +1156,10 @@
         <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1167,10 +1167,10 @@
         <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1178,10 +1178,10 @@
         <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1316,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
corrected bold text in dict
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yveswycisk/Library/Mobile Documents/com~apple~CloudDocs/HALT 2020/Veröffentlichung/Prozedur/Rohdaten - Fragen und Stimuli/V12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Documents\Wagner_3-0\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1649FDEB-D676-8843-B1CA-1C0C42D613A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45FC9BF-DD2D-4FF2-A312-E837061FAE55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21020" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="35844" windowHeight="21024" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -444,62 +444,62 @@
     <t>&lt;h4&gt;Wie viele Töne können Sie hören?&lt;/h4&gt;Ihre Aufgabe ist es wieder, **nur die gehörten Töne zu zählen** und den Zahlenwert in das Textfeld einzutragen. **Das Rauschen lassen Sie dabei unbeachtet und zählen es auch nicht mit**.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;Your task is **to count again only the tones heard ** and to enter the numerical value in the input box. **You should ignore the noise and not count it**.
+    <t>Der ERSTE Ton is am LEISESTEN.</t>
+  </si>
+  <si>
+    <t>Der ZWEIT Ton is am LEISESTEN.</t>
+  </si>
+  <si>
+    <t>Der DRITTE Ton is am LEISESTEN.</t>
+  </si>
+  <si>
+    <t>The FIRST sound is the SOFTEST.</t>
+  </si>
+  <si>
+    <t>The SECOND sound is the SOFTEST.</t>
+  </si>
+  <si>
+    <t>The THIRD sound is the SOFTEST.</t>
+  </si>
+  <si>
+    <t>Regularly from the left to the right or the right to the left</t>
+  </si>
+  <si>
+    <t>Irregular between the two channels</t>
+  </si>
+  <si>
+    <t>The tone moves from the right to the left side and back to the right side again.</t>
+  </si>
+  <si>
+    <t>The tone can only be heard on the left.</t>
+  </si>
+  <si>
+    <t>The tone can only be heard on the right.</t>
+  </si>
+  <si>
+    <t>Slowly from right to left.</t>
+  </si>
+  <si>
+    <t>Der Ton ist nur rechts zu hören.</t>
+  </si>
+  <si>
+    <t>Der Ton ist nur links zu hören.</t>
+  </si>
+  <si>
+    <t>Der Ton wandert von rechts nach links und anschließend wieder zurück nach rechts.</t>
+  </si>
+  <si>
+    <t>Der Ton wandert von links nach rechts und anschließend wieder zurück nach links.</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;When you click the play button, you will hear short noise events at regular intervals. In addition to the noise, tones are present. Tones and noise never sound simultaneously. Please **count only the tones heard** and enter the numerical value in the input box. **You should ignore the noise and not count it**.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;Your task is **to count again only the tones heard** and to enter the numerical value in the input box. **You should ignore the noise and not count it**.
 </t>
   </si>
   <si>
-    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;Your task is **to count again only the tones heard ** and to enter the numerical value in the input box. **You should ignore the noise and not count it**.</t>
-  </si>
-  <si>
-    <t>Der ERSTE Ton is am LEISESTEN.</t>
-  </si>
-  <si>
-    <t>Der ZWEIT Ton is am LEISESTEN.</t>
-  </si>
-  <si>
-    <t>Der DRITTE Ton is am LEISESTEN.</t>
-  </si>
-  <si>
-    <t>The FIRST sound is the SOFTEST.</t>
-  </si>
-  <si>
-    <t>The SECOND sound is the SOFTEST.</t>
-  </si>
-  <si>
-    <t>The THIRD sound is the SOFTEST.</t>
-  </si>
-  <si>
-    <t>Regularly from the left to the right or the right to the left</t>
-  </si>
-  <si>
-    <t>Irregular between the two channels</t>
-  </si>
-  <si>
-    <t>The tone moves from the right to the left side and back to the right side again.</t>
-  </si>
-  <si>
-    <t>The tone can only be heard on the left.</t>
-  </si>
-  <si>
-    <t>The tone can only be heard on the right.</t>
-  </si>
-  <si>
-    <t>Slowly from right to left.</t>
-  </si>
-  <si>
-    <t>Der Ton ist nur rechts zu hören.</t>
-  </si>
-  <si>
-    <t>Der Ton ist nur links zu hören.</t>
-  </si>
-  <si>
-    <t>Der Ton wandert von rechts nach links und anschließend wieder zurück nach rechts.</t>
-  </si>
-  <si>
-    <t>Der Ton wandert von links nach rechts und anschließend wieder zurück nach links.</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;When you click the play button, you will hear short noise events at regular intervals. In addition to the noise, tones are present. Tones and noise never sound simultaneously. Please **count only the tones heard** and enter the numerical value in the input box. **You should ignore the noise and not count it**.</t>
+    <t>&lt;h4&gt;How many tones can you hear?&lt;/h4&gt;Your task is **to count again only the tones heard** and to enter the numerical value in the input box. **You should ignore the noise and not count it**.</t>
   </si>
 </sst>
 </file>
@@ -865,18 +865,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="183.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="183.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="255.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="110" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -898,7 +898,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -909,7 +909,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -920,7 +920,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -931,7 +931,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -942,7 +942,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -953,7 +953,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -964,7 +964,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -972,10 +972,10 @@
         <v>134</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -983,10 +983,10 @@
         <v>135</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -994,10 +994,10 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1005,10 +1005,10 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1060,10 +1060,10 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1071,10 +1071,10 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1093,54 +1093,54 @@
         <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
@@ -1151,40 +1151,40 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>61</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>120</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>100</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>101</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>102</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>103</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>105</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>106</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
added non-formal German dict
</commit_message>
<xml_diff>
--- a/data_raw/HLT_dict.xlsx
+++ b/data_raw/HLT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Documents\Wagner_3-0\HALT\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kilian\Documents\HALT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85BC5F6-7208-4EE9-8C11-AF32A83097DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5B8620-E62D-4E47-BF03-F536970D964B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="35844" windowHeight="21024" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="0" yWindow="510" windowWidth="35850" windowHeight="21030" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="172">
   <si>
     <t>de</t>
   </si>
@@ -319,9 +319,6 @@
     <t>THLT_0013_CHOICES3</t>
   </si>
   <si>
-    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Kopfhörer zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Kopfhörern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmern wirklich Kopfhörer getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Kopfhörer zu tragen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Kopfhörer tragen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;You indicated that you are using a device different from headphones to reproduce sound. However, the use of headphones is a basic requirement for this survey.&lt;/p&gt;&lt;p&gt;We integrated special listening tasks in the further course of the questionnaire. These tasks check whether the participants are actually wearing headphones. &lt;/p&gt;&lt;p&gt;We therefore ask you &lt;strong&gt; to wear headphones from now on&lt;/strong&gt; to successfully complete the survey. If you do not wear headphones from now on, you will be automatically screened out during the survey. Given the length of the questionnaire, this would be a pity.&lt;/p&gt;</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
   </si>
   <si>
     <t>SCC_PROMPT_HP</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Lautsprecher zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Lautsprechern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmern wirklich Lautsprecher getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Lautsprecher zu benutzen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Lautsprecher benutzen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;You indicated that you are using a device different from loudspeakers to reproduce sound. However, the use of loudspeakers is a basic requirement for this survey.&lt;/p&gt;&lt;p&gt;We integrated special listening tasks in the further course of the questionnaire. These tasks check whether the participants are actually using loudspeakers. &lt;/p&gt;&lt;p&gt;We therefore ask you &lt;strong&gt; to use loudspeakers from now on&lt;/strong&gt; to successfully complete the survey. If you do not use loudspeakers from now on, you will be automatically screened out during the survey. Given the length of the questionnaire, this would be a pity.&lt;/p&gt;</t>
@@ -416,10 +410,6 @@
     <t>A circle and a triangle are shown in the picture. Is the circle located to the left or right of the triangle?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h4&gt;Wie viele Rausch-Abschnitte können Sie auf dem rechten Kopfhörer oder Lautsprecher hören?&lt;/h4&gt;Wenn Sie auf den Play-Button klicken, hören Sie sowohl auf dem linken, als auch auf dem rechten Kanal Rausch-Abschnitte. Bitte zählen Sie alle Rauschabschnitte, die Sie auf dem **rechten Kopfhörer oder Lautsprecher** wahrnehmen können und tragen Sie die Zahl in das Eingabefeld ein.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;h4&gt;How many noise events can you hear on the right headphone or loudspeaker?&lt;/h4&gt;When you click the play button, you will hear noise events on both the left and the right channel. Please count all noise events you can hear on the **right headphone or loudspeaker** and enter the number in the input box.
 </t>
   </si>
@@ -500,6 +490,70 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;h4&gt;Bitte stellen Sie die Wiedergabelautstärke entsprechend der Vorgaben ein.&lt;/h4&gt;Wenn Sie auf den Play-Button klicken, können Sie leise Rausch-Abschnitte hören. Bitte **stellen Sie die Wiedergabe-Lautstärke so ein**, dass Sie alle Rauschabschnitte **noch gerade eben hören können**. Dabei sollte die Einstellung so gewählt werden, dass Sie es nicht mehr hören könnten, wenn es etwas leiser wäre. </t>
+  </si>
+  <si>
+    <t>de_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Bitte stell die Wiedergabelautstärke entsprechend der Vorgaben ein.&lt;/h4&gt;Wenn Du auf den Play-Button klickst, kannst du leise Rausch-Abschnitte hören. Bitte **stell die Wiedergabe-Lautstärke so ein**, dass Du alle Rauschabschnitte **noch gerade eben hören kannst**. Dabei sollte die Einstellung so gewählt werden, dass Du es nicht mehr hören könntest, wenn es etwas leiser wäre. </t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Wie viele Rauschabschnitte kannst Du hören?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du ein kurzes Audiobeispiel, in dem leise und laute Abschnitte von einem Rauschen zu hören sind. Bitte  **zähle alle leisen und lauten Rauschabschnitte**  und trage den Zahlenwert in das Textfeld ein.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Wie viele Rauschabschnitte kannst Du hören?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du ein kurzes Audiobeispiel in dem leise und laute Abschnitte von einem Rauschen zu hören sind. Bitte  **zähle alle leisen und lauten Rauschabschnitte**  und trage den Zahlenwert in das Textfeld ein.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Wie viele Rausch-Abschnitte kannst Du auf dem rechten Kopfhörer oder Lautsprecher hören?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du sowohl auf dem linken, als auch auf dem rechten Kanal Rausch-Abschnitte. Bitte zähle alle Rauschabschnitte, die Du auf dem **rechten Kopfhörer oder Lautsprecher** wahrnehmen kannst, und trage die Zahl in das Eingabefeld ein.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Wie viele Rausch-Abschnitte können Sie auf dem rechten Kopfhörer oder Lautsprecher hören?&lt;/h4&gt;Wenn Sie auf den Play-Button klicken, hören Sie sowohl auf dem linken, als auch auf dem rechten Kanal Rausch-Abschnitte. Bitte zählen Sie alle Rauschabschnitte, die Sie auf dem **rechten Kopfhörer oder Lautsprecher** wahrnehmen können, und tragen Sie die Zahl in das Eingabefeld ein.
+</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Wie bewegt sich das Rauschen?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du ein Rauschsignal, das die wahrgenommene Position über die Zeit verändert. Das Rauschen scheint sich zu bewegen. Wie würdest Du diese Bewegung beschreiben?</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Wo kannst Du das Gehörte lokalisieren?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du einen Ton. Bitte gib an, wo Du den Ton lokalisieren kannst.</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Wie viele Töne kannst Du hören?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du kurze Rauschabschnitte in regelmäßigen Abständen. Neben dem Rauschen sind auch Töne zu hören, die jedoch nie gleichzeitig mit dem Rauschen erklingen. Bitte **zähle nur die gehörten Töne** und trage den Zahlenwert in das Textfeld ein. **Das Rauschen lässt Du dabei unbeachtet und zählst es auch nicht mit**.</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Welcher Ton ist am leisesten?&lt;/h4&gt;Wenn Du auf den Play-Button klickst, hörst Du ein Audiobeispiel, in dem drei Töne zu hören sind. Diese Töne sind durch kurze Pausen getrennt. Du sollst angeben, welcher Ton für Dich am leisesten klang.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie Ihre ID ein</t>
+  </si>
+  <si>
+    <t>Deine Eingabe war leider falsch. Bitte wiederhole die Aufgabe. Versuche dabei bitte genauer hinzuhören.</t>
+  </si>
+  <si>
+    <t>Deine Eingabe war leider falsch. Die Wiedergabelautstärke ist vermutlich zu gering. Du kannst die Lautstärke um einen kleinstmöglichen Wert erhöhen und danach die Aufgabe wiederholen.</t>
+  </si>
+  <si>
+    <t>die Befragung wurde beendet. Das kann mehrere Gründe haben:&lt;ol&gt;&lt;li&gt;Es haben bereits genügend Probanden mit einem ähnlichen Wiedergabegerät teilgenommen.&lt;/li&gt;&lt;li&gt; Dein Wiedergabegerät ist nicht Teil unserer Zielgruppe.&lt;/li&gt;
+&lt;/ol&gt;Da zukünftige Untersuchungen vielleicht mehr Probanden und andere Zielgruppen erfordern, würden wir uns freuen, Dich in der nächsten Studie wieder begrüßen zu können. \\Wir bedanken uns für Dein Interesse und Deine Teilnahme.</t>
+  </si>
+  <si>
+    <t>Deine Eingabe war leider falsch. Bitte wiederhole die Aufgabe.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Du hast angegeben, dass Du ein anderes Gerät als Kopfhörer zur Tonwiedergabe nutzt. Für diese Befragung ist die Nutzung von Kopfhörern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmenden wirklich Kopfhörer getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Dich daher &lt;strong&gt;AB jetzt unbedingt Kopfhörer zu tragen&lt;/strong&gt;, damit Du die Befragung erfolgreich abschließen kannst. Falls Du ab jetzt keine Kopfhörer trägst, wirst Du im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Kopfhörer zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Kopfhörern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmenden wirklich Kopfhörer getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Kopfhörer zu tragen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Kopfhörer tragen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Über welches Gerät gibst Du den Ton in dieser Befragung wieder? &lt;/p&gt;&lt;p&gt;Beispiel: Wenn Du ein Smartphone benutzt, das Du mit Kopfhörern verbunden hast, dann musst Du „Kopfhörer“ auswählen.&lt;/p&gt;&lt;p&gt;Wähle das am ehesten Zutreffende aus.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Du hast angegeben, dass Du ein anderes Gerät als Lautsprecher zur Tonwiedergabe nutzt. Für diese Befragung ist die Nutzung von Lautsprechern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmenden wirklich Lautsprecher benutzt werden.&lt;/p&gt;&lt;p&gt;Wir bitten Dich daher &lt;strong&gt;AB jetzt unbedingt Lautsprecher zu benutzen&lt;/strong&gt;, damit Du die Befragung erfolgreich abschließen kannst. Falls Du ab jetzt keine Lautsprecher benutzt, wirst Du im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sie haben angegeben, dass Sie ein anderes Gerät als Lautsprecher zur Tonwiedergabe nutzen. Für diese Befragung ist die Nutzung von Lautsprechern jedoch Grundvoraussetzung.&lt;/p&gt;&lt;p&gt;Im weiteren Verlauf des Fragebogens wurden spezielle Höraufgaben integriert. Mit diesen Aufgaben wird überprüft, ob von den Teilnehmenden wirklich Lautsprecher getragen werden.&lt;/p&gt;&lt;p&gt;Wir bitten Sie daher &lt;strong&gt;AB jetzt unbedingt Lautsprecher zu benutzen&lt;/strong&gt;, damit Sie die Befragung erfolgreich abschließen können. Falls Sie ab jetzt keine Lautsprecher benutzen, werden Sie im Verlauf der Befragung automatisch aussortiert. In Anbetracht der Länge der Befragung wäre dies sehr ärgerlich.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -863,20 +917,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="183.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="255.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="183.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -884,142 +938,181 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1027,10 +1120,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1038,10 +1134,13 @@
         <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1049,10 +1148,13 @@
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1060,21 +1162,27 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1082,10 +1190,13 @@
         <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1093,98 +1204,125 @@
         <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
@@ -1192,10 +1330,13 @@
         <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -1205,8 +1346,11 @@
       <c r="C30" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1214,10 +1358,13 @@
         <v>46</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1225,10 +1372,13 @@
         <v>45</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1236,10 +1386,13 @@
         <v>42</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1247,32 +1400,41 @@
         <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
@@ -1280,10 +1442,13 @@
         <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>61</v>
       </c>
@@ -1291,10 +1456,13 @@
         <v>62</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
@@ -1304,8 +1472,11 @@
       <c r="C39" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1313,21 +1484,27 @@
         <v>73</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -1335,10 +1512,13 @@
         <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
@@ -1346,117 +1526,150 @@
         <v>87</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>